<commit_message>
Completed up to line 30
</commit_message>
<xml_diff>
--- a/Abkhazia_Towns.xlsx
+++ b/Abkhazia_Towns.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22992" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="375">
   <si>
     <t>town_RU</t>
   </si>
@@ -1042,6 +1042,105 @@
   </si>
   <si>
     <t>41.28611</t>
+  </si>
+  <si>
+    <t>Чхәарҭал</t>
+  </si>
+  <si>
+    <t>42.754444</t>
+  </si>
+  <si>
+    <t>41.720833</t>
+  </si>
+  <si>
+    <t>Chkhortoli</t>
+  </si>
+  <si>
+    <t>Аибӷа</t>
+  </si>
+  <si>
+    <t>Aibgha</t>
+  </si>
+  <si>
+    <t>43.586111</t>
+  </si>
+  <si>
+    <t>40.198611</t>
+  </si>
+  <si>
+    <t>Ахьуара</t>
+  </si>
+  <si>
+    <t>43.238889</t>
+  </si>
+  <si>
+    <t>40.394722</t>
+  </si>
+  <si>
+    <t>Акәаскъа</t>
+  </si>
+  <si>
+    <t>42.795278</t>
+  </si>
+  <si>
+    <t>41.541111</t>
+  </si>
+  <si>
+    <t>Алакумхара</t>
+  </si>
+  <si>
+    <t>42.685278</t>
+  </si>
+  <si>
+    <t>41.912222</t>
+  </si>
+  <si>
+    <t>Алаҳаӡы</t>
+  </si>
+  <si>
+    <t>Alakhadzi</t>
+  </si>
+  <si>
+    <t>43.222222</t>
+  </si>
+  <si>
+    <t>40.297778</t>
+  </si>
+  <si>
+    <t>Амхял</t>
+  </si>
+  <si>
+    <t>43.036389</t>
+  </si>
+  <si>
+    <t>41.158611</t>
+  </si>
+  <si>
+    <t>Ачипста</t>
+  </si>
+  <si>
+    <t>Alpuri</t>
+  </si>
+  <si>
+    <t>43.283611</t>
+  </si>
+  <si>
+    <t>40.28</t>
+  </si>
+  <si>
+    <t>43.193056</t>
+  </si>
+  <si>
+    <t>40.407778</t>
+  </si>
+  <si>
+    <t>Амжәықәхәа</t>
+  </si>
+  <si>
+    <t>43.017222</t>
+  </si>
+  <si>
+    <t>41.35</t>
   </si>
 </sst>
 </file>
@@ -1469,21 +1568,21 @@
   <dimension ref="A1:H243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
     <col min="3" max="3" width="43" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="7" customWidth="1"/>
     <col min="8" max="8" width="22" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1512,7 +1611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -1538,7 +1637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
@@ -1564,7 +1663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
@@ -1590,7 +1689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
@@ -1616,7 +1715,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
@@ -1642,7 +1741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>72</v>
       </c>
@@ -1668,7 +1767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>62</v>
       </c>
@@ -1694,7 +1793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>74</v>
       </c>
@@ -1720,7 +1819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
@@ -1746,7 +1845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>68</v>
       </c>
@@ -1772,7 +1871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>312</v>
       </c>
@@ -1795,7 +1894,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>315</v>
       </c>
@@ -1818,7 +1917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>319</v>
       </c>
@@ -1842,7 +1941,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>326</v>
       </c>
@@ -1856,7 +1955,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>323</v>
       </c>
@@ -1880,7 +1979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>328</v>
       </c>
@@ -1903,7 +2002,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>330</v>
       </c>
@@ -1923,7 +2022,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>334</v>
       </c>
@@ -1949,7 +2048,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>336</v>
       </c>
@@ -1975,7 +2074,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>340</v>
       </c>
@@ -2001,39 +2100,143 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>349</v>
+      </c>
       <c r="C22" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>352</v>
+      </c>
       <c r="C23" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>355</v>
+      </c>
       <c r="C24" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>358</v>
+      </c>
       <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>362</v>
+      </c>
       <c r="C26" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="C27" s="5" t="s">
         <v>317</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>363</v>
+      </c>
       <c r="F27" s="15" t="s">
         <v>39</v>
       </c>
@@ -2042,24 +2245,71 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>369</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>371</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>374</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>318</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>318</v>
+      </c>
       <c r="F30" s="15" t="s">
         <v>39</v>
       </c>
@@ -2068,437 +2318,437 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C113" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C114" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C115" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C116" s="5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>299</v>
       </c>
@@ -2518,7 +2768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>303</v>
       </c>
@@ -2538,172 +2788,190 @@
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C119" s="5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C120" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C121" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C122" s="5" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C123" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C124" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C125" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C126" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C127" s="5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C128" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C129" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C130" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C131" s="5" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C132" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C133" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>358</v>
+      </c>
       <c r="C134" s="5" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H134" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C135" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C136" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C137" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C138" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C139" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C140" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C141" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C142" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C143" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C144" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C145" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C146" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C147" s="5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C148" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C149" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C150" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C151" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C152" s="5" t="s">
         <v>306</v>
       </c>
@@ -2714,292 +2982,292 @@
         <v>39</v>
       </c>
     </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C153" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C154" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C155" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C156" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C157" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C158" s="5" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C159" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C160" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C161" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C162" s="5" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C163" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C164" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C165" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C166" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C167" s="5" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C168" s="5" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C169" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C170" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C171" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C172" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C173" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C174" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C175" s="5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C176" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C177" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C178" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C179" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C180" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C181" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C182" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C183" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C184" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C185" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C187" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C188" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C189" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C190" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C191" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C192" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C193" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C194" s="5" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C195" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C196" s="5" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C197" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C198" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C199" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C200" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C201" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C202" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C203" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C204" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C205" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C206" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C207" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C208" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C209" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C210" s="5" t="s">
         <v>308</v>
       </c>
@@ -3010,7 +3278,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="211" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C211" s="5" t="s">
         <v>309</v>
       </c>
@@ -3021,82 +3289,82 @@
         <v>39</v>
       </c>
     </row>
-    <row r="212" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C212" s="5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C213" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C214" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C215" s="5" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C216" s="5" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="217" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C217" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C218" s="5" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="219" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C219" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="220" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C220" s="5" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="221" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C221" s="5" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="222" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C222" s="5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C223" s="5" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="224" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C224" s="5" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C225" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C226" s="5" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="227" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C227" s="5" t="s">
         <v>310</v>
       </c>
@@ -3107,7 +3375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C228" s="5" t="s">
         <v>311</v>
       </c>
@@ -3118,77 +3386,98 @@
         <v>39</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C229" s="5" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C230" s="5" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C231" s="5" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C232" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A233" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>344</v>
+      </c>
       <c r="C233" s="5" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D233" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E233" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F233" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G233" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H233" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C234" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="235" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C235" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C236" s="5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="237" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C237" s="5" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="238" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C238" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="239" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C239" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="240" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C240" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" s="5" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" s="5" t="s">
         <v>297</v>
       </c>
@@ -3205,7 +3494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3217,7 +3506,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed all towns starting with A
</commit_message>
<xml_diff>
--- a/Abkhazia_Towns.xlsx
+++ b/Abkhazia_Towns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="417">
   <si>
     <t>town_RU</t>
   </si>
@@ -309,12 +309,6 @@
     <t>Аракич</t>
   </si>
   <si>
-    <t>Арасадзых (Гагрский район)</t>
-  </si>
-  <si>
-    <t>Арасадзых (Очамчирский район)</t>
-  </si>
-  <si>
     <t>Арасара</t>
   </si>
   <si>
@@ -336,12 +330,6 @@
     <t>Ациджква</t>
   </si>
   <si>
-    <t>Ачандара (Гудаутский район)</t>
-  </si>
-  <si>
-    <t>Ачандара (Гульрипшский район)</t>
-  </si>
-  <si>
     <t>Ачгуара</t>
   </si>
   <si>
@@ -1141,6 +1129,144 @@
   </si>
   <si>
     <t>41.35</t>
+  </si>
+  <si>
+    <t>Амткял</t>
+  </si>
+  <si>
+    <t>43.03417</t>
+  </si>
+  <si>
+    <t>41.32444</t>
+  </si>
+  <si>
+    <t>Анхәа</t>
+  </si>
+  <si>
+    <t>43.11917</t>
+  </si>
+  <si>
+    <t>40.81222</t>
+  </si>
+  <si>
+    <t>41.4635</t>
+  </si>
+  <si>
+    <t>42.7730</t>
+  </si>
+  <si>
+    <t>Аракьаҽы</t>
+  </si>
+  <si>
+    <t>42.8437</t>
+  </si>
+  <si>
+    <t>41.2522</t>
+  </si>
+  <si>
+    <t>Арасаӡыхь</t>
+  </si>
+  <si>
+    <t>Арасадзых</t>
+  </si>
+  <si>
+    <t>43.23111</t>
+  </si>
+  <si>
+    <t>40.34278</t>
+  </si>
+  <si>
+    <t>42.88757</t>
+  </si>
+  <si>
+    <t>41.59553</t>
+  </si>
+  <si>
+    <t>43.09194</t>
+  </si>
+  <si>
+    <t>41.24806</t>
+  </si>
+  <si>
+    <t>43.05250</t>
+  </si>
+  <si>
+    <t>41.48583</t>
+  </si>
+  <si>
+    <t>Аҭара</t>
+  </si>
+  <si>
+    <t>42.89765</t>
+  </si>
+  <si>
+    <t>41.27776</t>
+  </si>
+  <si>
+    <t>Аҭара-Ерманқыҭ</t>
+  </si>
+  <si>
+    <t>42.90625</t>
+  </si>
+  <si>
+    <t>41.30923</t>
+  </si>
+  <si>
+    <t>Уадабаара</t>
+  </si>
+  <si>
+    <t>42.96000</t>
+  </si>
+  <si>
+    <t>41.21472</t>
+  </si>
+  <si>
+    <t>Аҭыдӡҭа</t>
+  </si>
+  <si>
+    <t>43.22472</t>
+  </si>
+  <si>
+    <t>40.38389</t>
+  </si>
+  <si>
+    <t>Ацыджкуа</t>
+  </si>
+  <si>
+    <t>43.20000</t>
+  </si>
+  <si>
+    <t>40.34306</t>
+  </si>
+  <si>
+    <t>Аҷандара</t>
+  </si>
+  <si>
+    <t>Ачандара</t>
+  </si>
+  <si>
+    <t>43.19333</t>
+  </si>
+  <si>
+    <t>40.72000</t>
+  </si>
+  <si>
+    <t>41.27611</t>
+  </si>
+  <si>
+    <t>Аҽгәара</t>
+  </si>
+  <si>
+    <t>42.68250</t>
+  </si>
+  <si>
+    <t>41.63361</t>
+  </si>
+  <si>
+    <t>43.42000</t>
+  </si>
+  <si>
+    <t>40.20222</t>
   </si>
 </sst>
 </file>
@@ -1567,9 +1693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1873,10 +1999,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>76</v>
@@ -1896,10 +2022,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>77</v>
@@ -1908,7 +2034,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>49</v>
@@ -1919,10 +2045,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>78</v>
@@ -1943,24 +2069,24 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>80</v>
@@ -1969,7 +2095,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>39</v>
@@ -1981,10 +2107,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>81</v>
@@ -1993,7 +2119,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>41</v>
@@ -2004,10 +2130,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>82</v>
@@ -2024,10 +2150,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>83</v>
@@ -2036,13 +2162,13 @@
         <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>42</v>
@@ -2050,10 +2176,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>84</v>
@@ -2068,7 +2194,7 @@
         <v>39</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>53</v>
@@ -2076,10 +2202,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>85</v>
@@ -2094,7 +2220,7 @@
         <v>39</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>53</v>
@@ -2102,10 +2228,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>86</v>
@@ -2114,13 +2240,13 @@
         <v>12</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>48</v>
@@ -2128,10 +2254,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>87</v>
@@ -2140,7 +2266,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>47</v>
@@ -2151,10 +2277,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>88</v>
@@ -2163,7 +2289,7 @@
         <v>14</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>54</v>
@@ -2174,10 +2300,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>89</v>
@@ -2186,7 +2312,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>25</v>
@@ -2197,10 +2323,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>90</v>
@@ -2209,13 +2335,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>48</v>
@@ -2223,19 +2349,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>39</v>
@@ -2247,10 +2373,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>91</v>
@@ -2259,13 +2385,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>48</v>
@@ -2273,10 +2399,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>92</v>
@@ -2285,7 +2411,7 @@
         <v>13</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>49</v>
@@ -2296,19 +2422,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>39</v>
@@ -2319,450 +2445,756 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>373</v>
+      </c>
       <c r="C31" s="5" t="s">
         <v>93</v>
       </c>
+      <c r="D31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>377</v>
+      </c>
       <c r="C33" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>381</v>
+      </c>
       <c r="C34" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>385</v>
+      </c>
       <c r="C35" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="5" t="s">
+      <c r="D37" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="5" t="s">
+      <c r="D38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="5" t="s">
+      <c r="D39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="5" t="s">
+      <c r="D40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="5" t="s">
+      <c r="D41" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="5" t="s">
+      <c r="D42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="5" t="s">
+      <c r="D43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="5" t="s">
+      <c r="D46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="5" t="s">
+      <c r="D47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C48" s="5" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="5" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C113" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C114" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C115" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C116" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F117" s="6" t="s">
         <v>39</v>
@@ -2770,19 +3202,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F118" s="6" t="s">
         <v>39</v>
@@ -2790,94 +3222,94 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C119" s="5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C120" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C121" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C122" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C123" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C124" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C125" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C126" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C127" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C128" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C129" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C130" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C131" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C132" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C133" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F134" s="6" t="s">
         <v>25</v>
@@ -2888,92 +3320,92 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C135" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C136" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C137" s="5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C138" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C139" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C140" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C141" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C142" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C143" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C144" s="5" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="145" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C145" s="5" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="146" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C146" s="5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C147" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C148" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="149" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C149" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C150" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C151" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C152" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>38</v>
@@ -2984,292 +3416,292 @@
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C153" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C154" s="5" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C155" s="5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="156" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C156" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C157" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C158" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C159" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C160" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C161" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C162" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C163" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C164" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C165" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C166" s="5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C167" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C168" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C169" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C170" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C171" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C172" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C173" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C174" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C175" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C176" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C177" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C178" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C179" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C180" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C181" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C182" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C183" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C184" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C185" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C187" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C188" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C189" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C190" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C191" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C192" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C193" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C194" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C195" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C196" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C197" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C198" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C199" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C200" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C201" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C202" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C203" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C204" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C205" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C206" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C207" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C208" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="209" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C209" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="210" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C210" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D210" s="5" t="s">
         <v>38</v>
@@ -3280,7 +3712,7 @@
     </row>
     <row r="211" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C211" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D211" s="5" t="s">
         <v>38</v>
@@ -3291,82 +3723,82 @@
     </row>
     <row r="212" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C212" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="213" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C213" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="214" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C214" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="215" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C215" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="216" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C216" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="217" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C217" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="218" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C218" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="219" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C219" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="220" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C220" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="221" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C221" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="222" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C222" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="223" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C223" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="224" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C224" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C225" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C226" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C227" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>38</v>
@@ -3377,7 +3809,7 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C228" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>38</v>
@@ -3388,45 +3820,45 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C229" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C230" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C231" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C232" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D233" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E233" s="6" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F233" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G233" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="H233" s="7" t="s">
         <v>51</v>
@@ -3434,52 +3866,52 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C234" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C235" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C236" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C237" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C238" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C239" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C240" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in 5 cities; removed 2 dupes
</commit_message>
<xml_diff>
--- a/Abkhazia_Towns.xlsx
+++ b/Abkhazia_Towns.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="430">
   <si>
     <t>town_RU</t>
   </si>
@@ -342,9 +342,6 @@
     <t>Бабышира</t>
   </si>
   <si>
-    <t>Багмарани</t>
-  </si>
-  <si>
     <t>Багмаран</t>
   </si>
   <si>
@@ -1267,6 +1264,48 @@
   </si>
   <si>
     <t>40.20222</t>
+  </si>
+  <si>
+    <t>42.86694</t>
+  </si>
+  <si>
+    <t>41.13278</t>
+  </si>
+  <si>
+    <t>Баҕмаран</t>
+  </si>
+  <si>
+    <t>43.00722</t>
+  </si>
+  <si>
+    <t>41.13222</t>
+  </si>
+  <si>
+    <t>Хышәҳарыҧшь</t>
+  </si>
+  <si>
+    <t>43.42806</t>
+  </si>
+  <si>
+    <t>40.14667</t>
+  </si>
+  <si>
+    <t>Баҕрыпсҭа</t>
+  </si>
+  <si>
+    <t>43.35694</t>
+  </si>
+  <si>
+    <t>40.13194</t>
+  </si>
+  <si>
+    <t>43.21611</t>
+  </si>
+  <si>
+    <t>40.49222</t>
+  </si>
+  <si>
+    <t>Бармышь</t>
   </si>
 </sst>
 </file>
@@ -1691,11 +1730,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H243"/>
+  <dimension ref="A1:H241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1999,10 +2038,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>309</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>76</v>
@@ -2022,10 +2061,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>312</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>77</v>
@@ -2034,7 +2073,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>49</v>
@@ -2045,10 +2084,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>316</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>78</v>
@@ -2069,24 +2108,24 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>320</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>80</v>
@@ -2095,7 +2134,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>39</v>
@@ -2107,10 +2146,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>325</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>81</v>
@@ -2119,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>41</v>
@@ -2130,10 +2169,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>326</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>327</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>82</v>
@@ -2150,10 +2189,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>331</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>83</v>
@@ -2162,13 +2201,13 @@
         <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>42</v>
@@ -2176,10 +2215,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>332</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>333</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>84</v>
@@ -2194,7 +2233,7 @@
         <v>39</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>53</v>
@@ -2202,10 +2241,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>336</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>337</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>85</v>
@@ -2220,7 +2259,7 @@
         <v>39</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>53</v>
@@ -2228,10 +2267,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>86</v>
@@ -2240,13 +2279,13 @@
         <v>12</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>48</v>
@@ -2254,10 +2293,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>348</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>87</v>
@@ -2266,7 +2305,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>47</v>
@@ -2277,10 +2316,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>350</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>351</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>88</v>
@@ -2289,7 +2328,7 @@
         <v>14</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>54</v>
@@ -2300,10 +2339,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>89</v>
@@ -2312,7 +2351,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>25</v>
@@ -2323,10 +2362,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>358</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>90</v>
@@ -2335,13 +2374,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>48</v>
@@ -2349,19 +2388,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>361</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>39</v>
@@ -2373,10 +2412,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>365</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>91</v>
@@ -2385,13 +2424,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>48</v>
@@ -2399,10 +2438,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>366</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>367</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>92</v>
@@ -2411,7 +2450,7 @@
         <v>13</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>49</v>
@@ -2422,19 +2461,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>370</v>
-      </c>
       <c r="C30" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>39</v>
@@ -2446,10 +2485,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>372</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>373</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>93</v>
@@ -2458,7 +2497,7 @@
         <v>38</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>39</v>
@@ -2469,10 +2508,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>376</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>94</v>
@@ -2481,7 +2520,7 @@
         <v>13</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>49</v>
@@ -2492,10 +2531,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>95</v>
@@ -2515,10 +2554,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>380</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>381</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>96</v>
@@ -2527,7 +2566,7 @@
         <v>14</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>54</v>
@@ -2538,19 +2577,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>385</v>
-      </c>
       <c r="C35" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>47</v>
@@ -2561,19 +2600,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>387</v>
-      </c>
       <c r="C36" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>54</v>
@@ -2584,10 +2623,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>97</v>
@@ -2607,10 +2646,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>390</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>391</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>98</v>
@@ -2630,10 +2669,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>393</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>394</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>99</v>
@@ -2642,7 +2681,7 @@
         <v>14</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>54</v>
@@ -2653,10 +2692,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>397</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>100</v>
@@ -2665,7 +2704,7 @@
         <v>14</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>54</v>
@@ -2676,10 +2715,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>400</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>101</v>
@@ -2688,7 +2727,7 @@
         <v>38</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>39</v>
@@ -2699,10 +2738,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>403</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>102</v>
@@ -2711,7 +2750,7 @@
         <v>12</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>47</v>
@@ -2722,10 +2761,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>406</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>103</v>
@@ -2734,7 +2773,7 @@
         <v>12</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>47</v>
@@ -2745,19 +2784,19 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>410</v>
-      </c>
       <c r="C44" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>49</v>
@@ -2768,19 +2807,19 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>39</v>
@@ -2791,10 +2830,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>414</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>104</v>
@@ -2803,7 +2842,7 @@
         <v>14</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>54</v>
@@ -2814,10 +2853,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>105</v>
@@ -2836,566 +2875,662 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>417</v>
+      </c>
       <c r="C48" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>420</v>
+      </c>
       <c r="C49" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>423</v>
+      </c>
       <c r="C50" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>426</v>
+      </c>
       <c r="C51" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>428</v>
+      </c>
       <c r="C52" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C53" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C55" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C56" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C57" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C58" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C59" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C60" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C61" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C62" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C63" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C64" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C113" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C114" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>295</v>
+      </c>
       <c r="C115" s="5" t="s">
-        <v>173</v>
+        <v>293</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>299</v>
+      </c>
       <c r="C116" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="D117" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>300</v>
-      </c>
       <c r="C118" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C119" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C120" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C121" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C122" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C123" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C124" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C125" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C126" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C127" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C128" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C129" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C130" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C131" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>353</v>
+      </c>
       <c r="C132" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C133" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>354</v>
-      </c>
       <c r="C134" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E134" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="F134" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C135" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C136" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C137" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C138" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C139" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C140" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C141" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C142" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C143" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C144" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="145" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C145" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C146" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="147" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C147" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="148" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C148" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="149" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C149" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="150" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C150" s="5" t="s">
-        <v>206</v>
+        <v>301</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.3">
@@ -3405,513 +3540,497 @@
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C152" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D152" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F152" s="6" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C153" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C154" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C155" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="156" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C156" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C157" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C158" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="159" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C159" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C160" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C161" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C162" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C163" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C164" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C165" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C166" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C167" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C168" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C169" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C170" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C171" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C172" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C173" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C174" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C175" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C176" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C177" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C178" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C179" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C180" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C181" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C182" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C183" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C184" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C185" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C187" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C188" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C189" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C190" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C191" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C192" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="193" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C193" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C194" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="195" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C195" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="196" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C196" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="197" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C197" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="198" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C198" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="199" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C199" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="200" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C200" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="201" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C201" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="202" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C202" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="203" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C203" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="204" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C204" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="205" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C205" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="206" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C206" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="207" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C207" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="208" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C208" s="5" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C195" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C196" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C197" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C198" s="5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C199" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C200" s="5" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C201" s="5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C202" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C203" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C204" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C205" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C206" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C207" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C208" s="5" t="s">
-        <v>262</v>
+      <c r="D208" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F208" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="209" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C209" s="5" t="s">
-        <v>263</v>
+        <v>304</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F209" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="210" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C210" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D210" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F210" s="6" t="s">
-        <v>39</v>
+        <v>263</v>
       </c>
     </row>
     <row r="211" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C211" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="D211" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F211" s="6" t="s">
-        <v>39</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C212" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="213" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C213" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="214" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C214" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="215" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C215" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C216" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C217" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C218" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="219" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C219" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C220" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C221" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C222" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C223" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="224" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C224" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C225" s="5" t="s">
-        <v>277</v>
+        <v>305</v>
+      </c>
+      <c r="D225" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F225" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C226" s="5" t="s">
-        <v>278</v>
+        <v>306</v>
+      </c>
+      <c r="D226" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F226" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C227" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="D227" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F227" s="6" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C228" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D228" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F228" s="6" t="s">
-        <v>39</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C229" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C230" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A231" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>339</v>
+      </c>
       <c r="C231" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+      <c r="D231" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E231" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="F231" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G231" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="H231" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C232" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A233" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B233" s="4" t="s">
-        <v>340</v>
-      </c>
       <c r="C233" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D233" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E233" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="F233" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G233" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="H233" s="7" t="s">
-        <v>51</v>
+        <v>284</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C234" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C235" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C236" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C237" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C238" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C239" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C240" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" s="5" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C242" s="5" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C243" s="5" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>